<commit_message>
Refactoring nos micro serviços de batch, files, relatorios
</commit_message>
<xml_diff>
--- a/batch-micro-service/src/main/resources/Laboratórios.xlsx
+++ b/batch-micro-service/src/main/resources/Laboratórios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -37,25 +37,28 @@
     <t xml:space="preserve">Número</t>
   </si>
   <si>
-    <t xml:space="preserve">Unidade Pinheiros</t>
+    <t xml:space="preserve">Unidade Interlagos</t>
   </si>
   <si>
     <t xml:space="preserve">São Paulo</t>
   </si>
   <si>
-    <t xml:space="preserve">Pinheiros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Praça 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unidade Penha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cupa</t>
+    <t xml:space="preserve">Interlagos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sabará</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidade Primavera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primavera Interlagos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S/N</t>
   </si>
 </sst>
 </file>
@@ -165,16 +168,16 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="38.48"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -191,7 +194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -205,10 +208,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>123</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
@@ -221,8 +224,8 @@
       <c r="D3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>212</v>
+      <c r="E3" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>